<commit_message>
Budget and layout update
</commit_message>
<xml_diff>
--- a/Proposal/Proposal budget.xlsx
+++ b/Proposal/Proposal budget.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436418C4-9004-4ABE-BB30-D15839DA82FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>Item</t>
   </si>
@@ -129,9 +137,6 @@
     <t>WHR boiler</t>
   </si>
   <si>
-    <t>WHR turbine housing</t>
-  </si>
-  <si>
     <t>WHR turbine</t>
   </si>
   <si>
@@ -193,12 +198,66 @@
   </si>
   <si>
     <t>Adjusted Grand total</t>
+  </si>
+  <si>
+    <t>Turbine bearings</t>
+  </si>
+  <si>
+    <t>6153k78</t>
+  </si>
+  <si>
+    <t>Mcmaster, stainless steel sealed bearings</t>
+  </si>
+  <si>
+    <t>Flow divider</t>
+  </si>
+  <si>
+    <t>Stator</t>
+  </si>
+  <si>
+    <t>Rotor</t>
+  </si>
+  <si>
+    <t>12343-300-01</t>
+  </si>
+  <si>
+    <t>12343-300-02</t>
+  </si>
+  <si>
+    <t>Potentially expensive fabrication</t>
+  </si>
+  <si>
+    <t>Condenser heat sink</t>
+  </si>
+  <si>
+    <t>12343-200-01</t>
+  </si>
+  <si>
+    <t>Drive shaft</t>
+  </si>
+  <si>
+    <t>Shaft coupler</t>
+  </si>
+  <si>
+    <t>5395t611</t>
+  </si>
+  <si>
+    <t>Assembly cost above and beyond component costs</t>
+  </si>
+  <si>
+    <t>Turbine housing</t>
+  </si>
+  <si>
+    <t>Mass estimate</t>
+  </si>
+  <si>
+    <t>Total mass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -289,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -300,6 +359,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -309,6 +370,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -357,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,9 +454,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,6 +506,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -600,11 +698,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,12 +711,14 @@
     <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,16 +732,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,18 +760,23 @@
       <c r="D2" s="2">
         <v>49.28</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="10"/>
+      <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
-        <f>E2*D2</f>
+      <c r="G2" s="2">
+        <f>F2*D2</f>
         <v>197.12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="10">
+        <f>F2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -678,16 +789,21 @@
       <c r="D3" s="2">
         <v>14.72</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="10"/>
+      <c r="F3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
-        <f>E3*D3</f>
+      <c r="G3" s="2">
+        <f>F3*D3</f>
         <v>58.88</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H31" si="0">F3*E3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -700,18 +816,23 @@
       <c r="D4" s="2">
         <v>1.63</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="10"/>
+      <c r="F4" s="1">
         <v>8</v>
       </c>
-      <c r="F4" s="2">
-        <f>E4*D4</f>
+      <c r="G4" s="2">
+        <f>F4*D4</f>
         <v>13.04</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -720,16 +841,21 @@
       <c r="D5" s="2">
         <v>20</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F23" si="0">E5*D5</f>
+      <c r="E5" s="10"/>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G30" si="1">F5*D5</f>
         <v>20</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -738,16 +864,21 @@
       <c r="D6" s="2">
         <v>35</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -760,16 +891,21 @@
       <c r="D7" s="2">
         <v>387.5</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
         <v>387.5</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -782,16 +918,21 @@
       <c r="D8" s="2">
         <v>187.5</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
         <v>187.5</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -804,18 +945,23 @@
       <c r="D9" s="2">
         <v>200</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -828,18 +974,23 @@
       <c r="D10" s="2">
         <v>89.02</v>
       </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
         <v>89.02</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -852,18 +1003,23 @@
       <c r="D11" s="2">
         <v>458.18</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
         <v>458.18</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -876,18 +1032,23 @@
       <c r="D12" s="2">
         <v>248.5</v>
       </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
         <v>248.5</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -896,388 +1057,653 @@
       <c r="D13" s="2">
         <v>250</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2">
-        <v>75</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>715</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>715</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2">
-        <v>550</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>550</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <f>F15*D15</f>
+        <v>75</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2">
-        <v>450</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46.32</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>92.64</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2">
-        <v>300</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2">
-        <v>100</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="2">
-        <v>105</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>420</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2">
-        <v>40</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2">
-        <v>30</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17.07</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>17.07</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2">
-        <v>150</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>415</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2">
-        <v>450</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5">
-        <f>SUM(F2:F24)</f>
-        <v>4789.74</v>
-      </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2">
+        <v>300</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2">
+        <v>100</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="2">
-        <f>F25*0.06</f>
-        <v>287.38439999999997</v>
-      </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="6">
-        <v>25</v>
-      </c>
-      <c r="E27" s="3">
-        <v>13</v>
-      </c>
-      <c r="F27" s="6">
-        <f>E27*D27</f>
-        <v>325</v>
-      </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5">
-        <f>SUM(F25:F27)</f>
-        <v>5402.1243999999997</v>
-      </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="D26" s="2">
+        <v>105</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2">
+        <v>40</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="1">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2">
+        <v>30</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <v>150</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1">
-        <v>50</v>
-      </c>
-      <c r="E30" s="1">
-        <v>12</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" ref="F30:F31" si="1">E30*D30</f>
-        <v>600</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="D30" s="2">
+        <v>450</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3">
-        <v>25</v>
-      </c>
-      <c r="E31" s="3">
-        <v>12</v>
-      </c>
-      <c r="F31" s="6">
-        <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="5">
-        <f>SUM(F30:F31)</f>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5">
+        <f>SUM(G2:G31)</f>
+        <v>5154.45</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="2">
+        <f>G32*0.06</f>
+        <v>309.267</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="6">
+        <v>25</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="3">
+        <v>13</v>
+      </c>
+      <c r="G34" s="6">
+        <f>F34*D34</f>
+        <v>325</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5">
+        <f>SUM(G32:G34)</f>
+        <v>5788.7169999999996</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1">
+        <v>50</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1">
+        <v>12</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" ref="G37:G38" si="2">F37*D37</f>
+        <v>600</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <v>25</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>12</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5">
+        <f>SUM(G37:G38)</f>
         <v>900</v>
       </c>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="H39" s="5"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5">
+        <f>G39+G35</f>
+        <v>6688.7169999999996</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="5">
-        <f>F32+F28</f>
-        <v>6302.1243999999997</v>
-      </c>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="6">
+        <f>G41*D42</f>
+        <v>1337.7434000000001</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="6">
-        <f>F34*D35</f>
-        <v>1260.42488</v>
-      </c>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="9">
-        <f>F35+F34</f>
-        <v>7562.5492799999993</v>
-      </c>
-      <c r="G36" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="9">
+        <f>G42+G41</f>
+        <v>8026.4603999999999</v>
+      </c>
+      <c r="H43" s="9"/>
+      <c r="I43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1289,7 +1715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>